<commit_message>
Updated start year to 2016
</commit_message>
<xml_diff>
--- a/pyonsset2018/Benin/specsBenin.xlsx
+++ b/pyonsset2018/Benin/specsBenin.xlsx
@@ -16,12 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
-    <t>Pop2015</t>
-  </si>
-  <si>
-    <t>UrbanRatio2015</t>
-  </si>
-  <si>
     <t>UrbanRatioModelled</t>
   </si>
   <si>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>Benin</t>
+  </si>
+  <si>
+    <t>Pop2016</t>
+  </si>
+  <si>
+    <t>UrbanRatio2016</t>
   </si>
 </sst>
 </file>
@@ -462,100 +462,100 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>10880000</v>
+        <v>10872000</v>
       </c>
       <c r="C2">
-        <v>0.44</v>
+        <v>0.44395000000000001</v>
       </c>
       <c r="E2">
         <v>15507000</v>
@@ -594,7 +594,7 @@
         <v>50</v>
       </c>
       <c r="R2">
-        <v>0.31</v>
+        <v>0.41403000000000001</v>
       </c>
       <c r="T2">
         <v>5</v>

</xml_diff>

<commit_message>
Added productive uses for health and education
</commit_message>
<xml_diff>
--- a/pyonsset2018/Benin/specsBenin.xlsx
+++ b/pyonsset2018/Benin/specsBenin.xlsx
@@ -167,9 +167,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -464,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +558,7 @@
         <v>0.44395000000000001</v>
       </c>
       <c r="D2">
-        <v>0.44367991736487311</v>
+        <v>0.44367991736487372</v>
       </c>
       <c r="E2">
         <v>15507000</v>
@@ -570,7 +567,7 @@
         <v>0.51300000000000001</v>
       </c>
       <c r="G2">
-        <v>3101.484877281825</v>
+        <v>3101.4848772818259</v>
       </c>
       <c r="H2">
         <v>3.6</v>
@@ -585,7 +582,7 @@
         <v>2.7</v>
       </c>
       <c r="L2">
-        <v>0.19</v>
+        <v>0.1065</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -606,7 +603,7 @@
         <v>0.41403000000000001</v>
       </c>
       <c r="S2">
-        <v>0.41796037458691582</v>
+        <v>0.55249752902628602</v>
       </c>
       <c r="T2">
         <v>60</v>

</xml_diff>

<commit_message>
Latest updated input values
</commit_message>
<xml_diff>
--- a/pyonsset2018/Benin/specsBenin.xlsx
+++ b/pyonsset2018/Benin/specsBenin.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm.esa\Documents\GitHub\PyOnSSET\pyonsset2018\Benin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -100,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,12 +173,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -215,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,7 +258,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +590,7 @@
         <v>2.7</v>
       </c>
       <c r="L2">
-        <v>0.1065</v>
+        <v>0.19</v>
       </c>
       <c r="M2">
         <v>2000</v>

</xml_diff>

<commit_message>
Updated with latest Specs and Settlements file
</commit_message>
<xml_diff>
--- a/pyonsset2018/Benin/specsBenin.xlsx
+++ b/pyonsset2018/Benin/specsBenin.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm.esa\Documents\GitHub\PyOnSSET\pyonsset2018\Benin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -105,8 +100,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,14 +164,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -223,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,10 +242,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,7 +276,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,16 +451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -555,7 +538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -563,25 +546,25 @@
         <v>10872000</v>
       </c>
       <c r="C2">
-        <v>0.44395000000000001</v>
+        <v>0.44395</v>
       </c>
       <c r="D2">
-        <v>0.44367991736487372</v>
+        <v>0.4436799173648737</v>
       </c>
       <c r="E2">
         <v>15507000</v>
       </c>
       <c r="F2">
-        <v>0.51300000000000001</v>
+        <v>0.513</v>
       </c>
       <c r="G2">
-        <v>3101.4848772818259</v>
+        <v>3101.484877281826</v>
       </c>
       <c r="H2">
-        <v>3.6</v>
+        <v>6</v>
       </c>
       <c r="I2">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="J2">
         <v>1.04</v>
@@ -590,7 +573,7 @@
         <v>2.7</v>
       </c>
       <c r="L2">
-        <v>0.19</v>
+        <v>0.1322</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -608,10 +591,10 @@
         <v>50</v>
       </c>
       <c r="R2">
-        <v>0.41403000000000001</v>
+        <v>0.29</v>
       </c>
       <c r="S2">
-        <v>0.55249752902628602</v>
+        <v>0.5523046117685825</v>
       </c>
       <c r="T2">
         <v>60</v>

</xml_diff>